<commit_message>
minor updates to chart
</commit_message>
<xml_diff>
--- a/glasgow_simd_msoa_2020_charts_elec_gas.xlsx
+++ b/glasgow_simd_msoa_2020_charts_elec_gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\Una\DataSkills\Projects\EPC_SIMD_MSOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CAE537-AA87-46B4-9305-043CB56BA7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B5D68-BFCA-4E1E-A7FD-E2463CAFAE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="911" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2103,7 +2103,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>reas of high and low income deprivation</a:t>
+              <a:t>reas of high and low income deprivation, Glasgow</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -10689,7 +10689,7 @@
       <cdr:y>0.27316</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.85741</cdr:x>
+      <cdr:x>0.88975</cdr:x>
       <cdr:y>0.3941</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -10705,8 +10705,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8956675" y="1441450"/>
-          <a:ext cx="1333500" cy="638175"/>
+          <a:off x="7589854" y="1441424"/>
+          <a:ext cx="1458895" cy="638182"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -11269,8 +11269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD59852-F26C-47A9-81DD-B2C7536F893F}">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11278,13 +11278,12 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="17" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="17" width="14.5703125" customWidth="1"/>
     <col min="18" max="18" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.140625" bestFit="1" customWidth="1"/>
@@ -11315,13 +11314,13 @@
       <c r="G1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">

</xml_diff>